<commit_message>
add book and excel chart
</commit_message>
<xml_diff>
--- a/drawChartInExcel/chart.xlsx
+++ b/drawChartInExcel/chart.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ChartSheet_0" sheetId="2" r:id="rId2"/>
+    <sheet name="ChartSheet_0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>thang</t>
   </si>
@@ -42,6 +41,9 @@
   </si>
   <si>
     <t>thang 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gia tri moi </t>
   </si>
 </sst>
 </file>
@@ -248,24 +250,25 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>ChartSheet_0!$B$1</c:f>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>ChartSheet_0!$A$2:$A$7</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>ChartSheet_0!$B$2:$B$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -275,27 +278,122 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>ChartSheet_0!$C$1</c:f>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>ChartSheet_0!$A$2:$A$7</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>ChartSheet_0!$C$2:$C$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="18274237"/>
+        <c:axId val="11396073"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="18274237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr anchor="ctr" rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr b="0" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" charset="0"/>
+                    <a:ea typeface="Calibri" charset="0"/>
+                    <a:cs typeface="Calibri" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>thoi gian</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="11396073"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11396073"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr anchor="ctr" rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr b="0" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" charset="0"/>
+                    <a:ea typeface="Calibri" charset="0"/>
+                    <a:cs typeface="Calibri" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>So luong da ban </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="18274237"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:srgbClr val="C0C0C0"/>
+        </a:solidFill>
         <a:ln w="9525">
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="808080"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -309,31 +407,28 @@
   <c:spPr>
     <a:ln w="9525"/>
   </c:spPr>
+  <c:printSettings>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetProtection/>
-  <pageMargins left="0.75" right="0.75" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1" name="Chart 1" descr="Chart 1"/>
@@ -350,7 +445,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:absoluteAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -640,9 +735,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15.0"/>
   <sheetData>
@@ -723,8 +818,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add cpp and download selenium test
</commit_message>
<xml_diff>
--- a/drawChartInExcel/chart.xlsx
+++ b/drawChartInExcel/chart.xlsx
@@ -294,11 +294,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="18274237"/>
-        <c:axId val="11396073"/>
+        <c:axId val="2696283"/>
+        <c:axId val="17959908"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18274237"/>
+        <c:axId val="2696283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,14 +336,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11396073"/>
+        <c:crossAx val="17959908"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11396073"/>
+        <c:axId val="17959908"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,7 +382,7 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18274237"/>
+        <c:crossAx val="2696283"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>